<commit_message>
Update alert and healing data with new entries
Adds new entries to `email_tracker.json`, `healing_history.json`, and `healing_notifications.json` for alerts and task reallocations.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e3da4e62-7465-400e-b685-c50e454d4877
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Event-Id: 835b4efe-4d05-4460-a54d-c732db9e0ac8
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/09196ed5-9ce0-4f16-9e9c-7235c49f147a/e3da4e62-7465-400e-b685-c50e454d4877/Eb8SXBG
</commit_message>
<xml_diff>
--- a/data/project_wbs.xlsx
+++ b/data/project_wbs.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L73"/>
+  <dimension ref="A1:N73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,6 +498,16 @@
           <t>dependencies</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>risk_level</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>risk_reason</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -550,6 +560,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -602,6 +622,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -654,6 +684,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>On schedule, 0% complete</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -706,6 +746,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -758,6 +808,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -810,6 +870,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -862,6 +932,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -914,6 +994,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -966,6 +1056,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1018,6 +1118,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1070,6 +1180,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1122,6 +1242,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1174,6 +1304,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1226,6 +1366,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>at_risk</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>Due Nov 27, progress: 20%</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1278,6 +1428,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1330,6 +1490,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>On schedule, 20% complete</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1382,6 +1552,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1434,6 +1614,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1486,6 +1676,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>On schedule, 70% complete</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1538,6 +1738,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>On schedule, 70% complete</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1590,6 +1800,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1642,6 +1862,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1694,6 +1924,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -1746,6 +1986,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -1798,6 +2048,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>On schedule, 20% complete</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -1850,6 +2110,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>On schedule, 40% complete</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -1902,6 +2172,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1954,6 +2234,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>alert</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>Due in 5 days (Nov 21), only 10% complete</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2006,6 +2296,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>at_risk</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>Due Nov 25, progress: 40%</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2058,6 +2358,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>On schedule, 60% complete</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2110,6 +2420,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2162,6 +2482,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2214,6 +2544,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>On schedule, 70% complete</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2266,6 +2606,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>On schedule, 50% complete</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2318,6 +2668,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>On schedule, 60% complete</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2370,6 +2730,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>at_risk</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>Due Nov 24, progress: 40%</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2422,6 +2792,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2474,6 +2854,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>alert</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>Due in 2 days (Nov 18), only 10% complete</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2526,6 +2916,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2578,6 +2978,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>On schedule, 10% complete</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -2630,6 +3040,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -2682,6 +3102,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2734,6 +3164,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2786,6 +3226,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2838,6 +3288,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>On schedule, 40% complete</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -2890,6 +3350,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -2942,6 +3412,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>On schedule, 60% complete</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -2994,6 +3474,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3046,6 +3536,16 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>On schedule, 50% complete</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3098,10 +3598,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>On schedule, 40% complete</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -3150,10 +3660,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>at_risk</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>Due Nov 29, progress: 40%</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -3202,10 +3722,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>On schedule, 70% complete</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -3254,10 +3784,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -3306,10 +3846,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -3358,10 +3908,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -3410,10 +3970,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>On schedule, 40% complete</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -3462,10 +4032,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>On schedule, 70% complete</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -3514,10 +4094,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -3566,10 +4156,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>On schedule, 15% complete</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -3618,10 +4218,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>On schedule, 15% complete</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -3670,10 +4280,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>On schedule, 15% complete</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -3722,10 +4342,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -3774,10 +4404,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>On schedule, 40% complete</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -3826,10 +4466,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -3878,10 +4528,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -3930,10 +4590,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>On schedule, 20% complete</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -3982,10 +4652,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -4034,10 +4714,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -4051,7 +4741,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>adarshprvt@gmail.com</t>
+          <t>adarsh.arvr@gmail.com</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -4061,7 +4751,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>adarshprvt@gmail.com</t>
+          <t>adarsh.arvr@gmail.com</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -4078,18 +4768,28 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>AUTO-REALLOCATED to adarsh.arvr@gmail.com</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
           <t>nan</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>alert</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>Due in 2 days (Nov 18), only 10% complete</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -4138,10 +4838,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -4190,10 +4900,20 @@
           <t>nan</t>
         </is>
       </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>Completed: 100%</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -4240,6 +4960,16 @@
       <c r="L73" t="inlineStr">
         <is>
           <t>nan</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>on_track</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>Not due this month</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add record of a task being reallocated due to deadline concerns
Adds a new entry to the healing history and notifications JSON files detailing the reallocation of a task from one email to another, along with associated metadata.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e3da4e62-7465-400e-b685-c50e454d4877
Replit-Commit-Checkpoint-Type: intermediate_checkpoint
Replit-Commit-Event-Id: a8c5d9ae-69d4-4bfd-b140-c8657c544086
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/09196ed5-9ce0-4f16-9e9c-7235c49f147a/e3da4e62-7465-400e-b685-c50e454d4877/Eb8SXBG
</commit_message>
<xml_diff>
--- a/data/project_wbs.xlsx
+++ b/data/project_wbs.xlsx
@@ -4741,7 +4741,7 @@
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>adarsh.arvr@gmail.com</t>
+          <t>adarshprvt@gmail.com</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -4751,7 +4751,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>adarsh.arvr@gmail.com</t>
+          <t>adarshprvt@gmail.com</t>
         </is>
       </c>
       <c r="G70" t="n">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>AUTO-REALLOCATED to adarsh.arvr@gmail.com</t>
+          <t>AUTO-REALLOCATED to adarshprvt@gmail.com</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">

</xml_diff>